<commit_message>
Add current operations and with private flex accounts.
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\ICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC443486-5B2D-49FF-AD64-5D6989F6016F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33C3F48-2F12-472F-BD53-D3AF66F2DF0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>CAWCD</t>
+  </si>
+  <si>
+    <t>US+MX</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,6 +666,7 @@
     <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" customWidth="1"/>
+    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -730,6 +734,9 @@
       <c r="L6" s="22" t="s">
         <v>53</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
@@ -774,6 +781,10 @@
       <c r="L7" s="20">
         <f t="shared" si="0"/>
         <v>41000</v>
+      </c>
+      <c r="N7" s="12">
+        <f>SUM(E7:F7)</f>
+        <v>3014329</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update key points slides.
</commit_message>
<xml_diff>
--- a/ICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/ICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33C3F48-2F12-472F-BD53-D3AF66F2DF0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C7EF9-F01F-4A35-8D93-47DC9FAB07CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,11 +662,11 @@
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -1421,14 +1421,14 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -1894,10 +1894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
-  <dimension ref="A2:I5"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+    <sheetView topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2022,6 +2022,12 @@
       <c r="I5" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F7" s="13">
+        <f>SUM(F3:F5)</f>
+        <v>55434</v>
       </c>
     </row>
   </sheetData>
@@ -2039,7 +2045,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>